<commit_message>
updated excel formulas commit
</commit_message>
<xml_diff>
--- a/results/question_01_score_analysis.xlsx
+++ b/results/question_01_score_analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashvinn\Documents\GitHub\LLM_Interpretability_Research\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashvi\PycharmProjects\LLM_Interpretability_Research\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3239390-3981-4594-9717-E6FC2CCCA17A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79040D3B-A498-427F-9C15-77EC7D3058AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{5E48FF71-2AC4-4518-9E04-3DE549F6596A}"/>
   </bookViews>
@@ -25,7 +25,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -132,7 +137,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -299,7 +304,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -326,12 +331,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -356,10 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -369,22 +366,8 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,7 +397,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:colOff>1162049</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
@@ -462,8 +445,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>981675</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>105046</xdr:rowOff>
     </xdr:to>
@@ -865,40 +848,40 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.75" style="8" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.25" customWidth="1"/>
-    <col min="8" max="8" width="1.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.25" customWidth="1"/>
-    <col min="10" max="10" width="12.375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.875" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.85546875" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="20"/>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="30" t="s">
         <v>14</v>
       </c>
@@ -914,9 +897,9 @@
       <c r="M2" s="30"/>
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
-      <c r="P2" s="29"/>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1">
+      <c r="P2" s="26"/>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -952,9 +935,9 @@
       <c r="O3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="23"/>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="Q3" s="20"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -977,10 +960,10 @@
         <f>SUM(B4:D4)/3</f>
         <v>0.57846621009469867</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="18">
         <v>2</v>
       </c>
-      <c r="I4" s="21"/>
+      <c r="I4" s="18"/>
       <c r="J4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1003,11 +986,11 @@
         <f>SUM(K4:M4)/3</f>
         <v>0.456450377566541</v>
       </c>
-      <c r="Q4" s="22">
+      <c r="Q4" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1030,10 +1013,10 @@
         <f t="shared" ref="G5:G12" si="0">SUM(B5:D5)/3</f>
         <v>0.41414976272354465</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="22">
         <v>9</v>
       </c>
-      <c r="I5" s="24"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1056,11 +1039,11 @@
         <f>SUM(K5:M5)/3</f>
         <v>0.29985818980833301</v>
       </c>
-      <c r="Q5" s="26">
+      <c r="Q5" s="23">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1083,10 +1066,10 @@
         <f t="shared" si="0"/>
         <v>0.43395975930726699</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="22">
         <v>8</v>
       </c>
-      <c r="I6" s="24"/>
+      <c r="I6" s="21"/>
       <c r="J6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1109,11 +1092,11 @@
         <f t="shared" ref="P6:P12" si="1">SUM(K6:M6)/3</f>
         <v>0.30924465214480701</v>
       </c>
-      <c r="Q6" s="26">
+      <c r="Q6" s="23">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1136,10 +1119,10 @@
         <f t="shared" si="0"/>
         <v>0.49904605443065658</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="18">
         <v>6</v>
       </c>
-      <c r="I7" s="21"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1162,11 +1145,11 @@
         <f t="shared" si="1"/>
         <v>0.37823283337021163</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="Q7" s="19">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1189,10 +1172,10 @@
         <f t="shared" si="0"/>
         <v>0.5348525346762717</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="18">
         <v>4</v>
       </c>
-      <c r="I8" s="21"/>
+      <c r="I8" s="18"/>
       <c r="J8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1215,12 +1198,12 @@
         <f t="shared" si="1"/>
         <v>0.38920584047789197</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="Q8" s="19">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="33" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="12">
@@ -1242,11 +1225,11 @@
         <f t="shared" si="0"/>
         <v>0.548354342002351</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="24">
         <v>3</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="33" t="s">
+      <c r="I9" s="18"/>
+      <c r="J9" s="29" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="12">
@@ -1268,11 +1251,11 @@
         <f t="shared" si="1"/>
         <v>0.44167461963680993</v>
       </c>
-      <c r="Q9" s="28">
+      <c r="Q9" s="25">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -1295,10 +1278,10 @@
         <f t="shared" si="0"/>
         <v>0.46346085160863471</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="18">
         <v>7</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="18"/>
       <c r="J10" s="5" t="s">
         <v>7</v>
       </c>
@@ -1321,11 +1304,11 @@
         <f t="shared" si="1"/>
         <v>0.36341910470826227</v>
       </c>
-      <c r="Q10" s="22">
+      <c r="Q10" s="19">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1348,10 +1331,10 @@
         <f t="shared" si="0"/>
         <v>0.52504323839140865</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="18">
         <v>5</v>
       </c>
-      <c r="I11" s="21"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1374,12 +1357,12 @@
         <f t="shared" si="1"/>
         <v>0.39924828152471936</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="19">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="33" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="12">
@@ -1401,11 +1384,11 @@
         <f t="shared" si="0"/>
         <v>0.58166365592027636</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="24">
         <v>1</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="33" t="s">
+      <c r="I12" s="18"/>
+      <c r="J12" s="29" t="s">
         <v>6</v>
       </c>
       <c r="K12" s="12">
@@ -1427,21 +1410,21 @@
         <f t="shared" si="1"/>
         <v>0.4844833482466413</v>
       </c>
-      <c r="Q12" s="28">
+      <c r="Q12" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="str">
         <f>INDEX($A4:$A12, MATCH(MAX(B4:B12), B4:B12, 0))</f>
         <v>v2-html</v>
       </c>
       <c r="C13" s="7" t="str">
-        <f t="shared" ref="C13:D13" si="2">INDEX($A4:$A12, MATCH(MAX(C4:C12), C4:C12, 0))</f>
+        <f>INDEX($A4:$A12, MATCH(MAX(C4:C12), C4:C12, 0))</f>
         <v>v0-unstruct</v>
       </c>
       <c r="D13" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>INDEX($A4:$A12, MATCH(MAX(D4:D12), D4:D12, 0))</f>
         <v>v2-toml</v>
       </c>
       <c r="E13" s="7"/>
@@ -1472,35 +1455,35 @@
         <v>v2-toml</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="1" customFormat="1">
+    <row r="17" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J17" s="10"/>
-      <c r="Q17" s="23"/>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="B18" s="17" t="s">
+      <c r="Q17" s="20"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
-      <c r="B19" s="17" t="s">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
-      <c r="B20" s="19" t="s">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>25</v>
       </c>
@@ -1548,45 +1531,45 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.25" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="11"/>
-      <c r="R1" s="22"/>
-    </row>
-    <row r="2" spans="1:18" ht="15">
+      <c r="R1" s="19"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="30" t="s">
         <v>14</v>
@@ -1603,10 +1586,10 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="22"/>
-    </row>
-    <row r="3" spans="1:18" ht="15">
+      <c r="Q2" s="26"/>
+      <c r="R2" s="19"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -1643,7 +1626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1666,10 +1649,10 @@
         <f>SUM(B4:E4)/3</f>
         <v>0.77936286743278094</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="18">
         <v>6</v>
       </c>
-      <c r="I4" s="21"/>
+      <c r="I4" s="18"/>
       <c r="J4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1692,11 +1675,11 @@
         <f>SUM(K4:N4)/3</f>
         <v>0.60280012264875393</v>
       </c>
-      <c r="Q4" s="22">
+      <c r="Q4" s="19">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1719,10 +1702,10 @@
         <f t="shared" ref="G5:G11" si="0">SUM(B5:E5)/3</f>
         <v>0.78932657339022605</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="18">
         <v>3</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="18"/>
       <c r="J5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1745,11 +1728,11 @@
         <f t="shared" ref="P5:P11" si="1">SUM(K5:N5)/3</f>
         <v>0.66418737130651662</v>
       </c>
-      <c r="Q5" s="27">
+      <c r="Q5" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1772,10 +1755,10 @@
         <f t="shared" si="0"/>
         <v>0.75474607600509847</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="27">
         <v>7</v>
       </c>
-      <c r="I6" s="21"/>
+      <c r="I6" s="18"/>
       <c r="J6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1798,12 +1781,12 @@
         <f t="shared" si="1"/>
         <v>0.54187788685196925</v>
       </c>
-      <c r="Q6" s="32">
+      <c r="Q6" s="28">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15">
-      <c r="A7" s="33" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="12">
@@ -1825,11 +1808,11 @@
         <f t="shared" si="0"/>
         <v>0.80171543250001809</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="24">
         <v>1</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="33" t="s">
+      <c r="I7" s="18"/>
+      <c r="J7" s="29" t="s">
         <v>16</v>
       </c>
       <c r="K7" s="12">
@@ -1851,11 +1834,11 @@
         <f t="shared" si="1"/>
         <v>0.65977591259017843</v>
       </c>
-      <c r="Q7" s="27">
+      <c r="Q7" s="24">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1878,10 +1861,10 @@
         <f t="shared" si="0"/>
         <v>0.79640615027046335</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="24">
         <v>2</v>
       </c>
-      <c r="I8" s="21"/>
+      <c r="I8" s="18"/>
       <c r="J8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1904,11 +1887,11 @@
         <f t="shared" si="1"/>
         <v>0.63231995541443997</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="Q8" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1931,10 +1914,10 @@
         <f t="shared" si="0"/>
         <v>0.78326403915571463</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="18">
         <v>5</v>
       </c>
-      <c r="I9" s="21"/>
+      <c r="I9" s="18"/>
       <c r="J9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1957,11 +1940,11 @@
         <f t="shared" si="1"/>
         <v>0.60306673621850104</v>
       </c>
-      <c r="Q9" s="22">
+      <c r="Q9" s="19">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1984,10 +1967,10 @@
         <f t="shared" si="0"/>
         <v>0.73930229579307494</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="27">
         <v>8</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="18"/>
       <c r="J10" s="5" t="s">
         <v>11</v>
       </c>
@@ -2010,11 +1993,11 @@
         <f t="shared" si="1"/>
         <v>0.55173734182836609</v>
       </c>
-      <c r="Q10" s="32">
+      <c r="Q10" s="28">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
@@ -2037,10 +2020,10 @@
         <f t="shared" si="0"/>
         <v>0.78396611169092612</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="18">
         <v>4</v>
       </c>
-      <c r="I11" s="21"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="5" t="s">
         <v>6</v>
       </c>
@@ -2063,105 +2046,80 @@
         <f t="shared" si="1"/>
         <v>0.61152803757907592</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="19">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="7" t="str">
-        <f>INDEX($A4:$A10, MATCH(MAX(B4:B10), B4:B10, 0))</f>
+        <f>INDEX($A4:$A11, MATCH(MAX(B4:B11), B4:B11, 0))</f>
         <v>v2-custom3</v>
       </c>
       <c r="C12" s="7" t="str">
-        <f>INDEX($A4:$A10, MATCH(MAX(C4:C10), C4:C10, 0))</f>
+        <f t="shared" ref="C12:E12" si="2">INDEX($A4:$A11, MATCH(MAX(C4:C11), C4:C11, 0))</f>
         <v>v2-json</v>
       </c>
       <c r="D12" s="7" t="str">
-        <f>INDEX($A4:$A10, MATCH(MAX(D4:D10), D4:D10, 0))</f>
+        <f t="shared" si="2"/>
         <v>v2-custom2</v>
       </c>
       <c r="E12" s="7" t="str">
-        <f>INDEX($A4:$A10, MATCH(MAX(E4:E10), E4:E10, 0))</f>
+        <f>INDEX($A4:$A11, MATCH(MAX(E4:E11), E4:E11, 0))</f>
         <v>v2-custom1</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="16" t="str">
-        <f>INDEX($A3:$A11, MATCH(MAX(G3:G11), G3:G11, 0))</f>
+        <f>INDEX($A4:$A11, MATCH(MAX(G4:G11), G4:G11, 0))</f>
         <v>v2-custom3</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="8"/>
       <c r="K12" s="7" t="str">
-        <f>INDEX($J4:$J10, MATCH(MAX(K4:K10), K4:K10, 0))</f>
+        <f>INDEX($J4:$J11, MATCH(MAX(K4:K11), K4:K11, 0))</f>
         <v>v2-custom3</v>
       </c>
       <c r="L12" s="7" t="str">
-        <f>INDEX($J4:$J10, MATCH(MAX(L4:L10), L4:L10, 0))</f>
-        <v>v2-custom3</v>
+        <f>INDEX($J4:$J11, MATCH(MAX(L4:L11), L4:L11, 0))</f>
+        <v>v2-toml</v>
       </c>
       <c r="M12" s="7" t="str">
-        <f>INDEX($J4:$J10, MATCH(MAX(M4:M10), M4:M10, 0))</f>
+        <f>INDEX($J4:$J11, MATCH(MAX(M4:M11), M4:M11, 0))</f>
         <v>v2-custom2</v>
       </c>
       <c r="N12" s="7" t="str">
-        <f>INDEX($J4:$J10, MATCH(MAX(N4:N10), N4:N10, 0))</f>
+        <f>INDEX($J4:$J11, MATCH(MAX(N4:N11), N4:N11, 0))</f>
         <v>v2-custom1</v>
       </c>
       <c r="O12" s="7"/>
       <c r="P12" s="16" t="str">
-        <f>INDEX($A3:$A11, MATCH(MAX(P3:P11), P3:P11, 0))</f>
+        <f>INDEX($J4:$J11, MATCH(MAX(P4:P11), P4:P11, 0))</f>
         <v>v2-custom1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="15" customHeight="1">
-      <c r="B17" s="17" t="s">
+    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="O17" s="17"/>
-    </row>
-    <row r="18" spans="2:15" ht="15" customHeight="1">
-      <c r="B18" s="18" t="s">
+    </row>
+    <row r="18" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-    </row>
-    <row r="19" spans="2:15" ht="15">
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>25</v>
       </c>
       <c r="K19" s="5"/>
     </row>
-    <row r="34" spans="2:2" ht="15">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
         <v>22</v>
       </c>
@@ -2174,8 +2132,8 @@
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="L2:P2"/>
   </mergeCells>
-  <conditionalFormatting sqref="K4:N11">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="B4:E11">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2186,8 +2144,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E11">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="K4:N11">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2208,30 +2166,30 @@
   <dimension ref="A2:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.125" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.875" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.875" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="30" t="s">
         <v>14</v>
@@ -2248,9 +2206,9 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
-      <c r="Q2" s="39"/>
-    </row>
-    <row r="3" spans="1:17" ht="15">
+      <c r="Q2" s="26"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -2268,7 +2226,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="36"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="9"/>
       <c r="K3" s="2" t="s">
@@ -2287,7 +2245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2307,13 +2265,13 @@
         <v>0</v>
       </c>
       <c r="G4" s="15">
-        <f>SUM(B4:E4)/3</f>
+        <f t="shared" ref="G4:G11" si="0">SUM(B4:E4)/3</f>
         <v>0.79287936412564131</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="18">
         <v>3</v>
       </c>
-      <c r="I4" s="21"/>
+      <c r="I4" s="18"/>
       <c r="J4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2333,14 +2291,14 @@
         <v>0</v>
       </c>
       <c r="P4" s="15">
-        <f>SUM(K4:N4)/3</f>
+        <f t="shared" ref="P4:P11" si="1">SUM(K4:N4)/3</f>
         <v>0.6175690066824463</v>
       </c>
-      <c r="Q4" s="40">
+      <c r="Q4" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -2360,13 +2318,13 @@
         <v>0</v>
       </c>
       <c r="G5" s="15">
-        <f>SUM(B5:E5)/3</f>
+        <f t="shared" si="0"/>
         <v>0.75614608743202327</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="27">
         <v>7</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="18"/>
       <c r="J5" s="5" t="s">
         <v>8</v>
       </c>
@@ -2386,14 +2344,14 @@
         <v>0</v>
       </c>
       <c r="P5" s="15">
-        <f>SUM(K5:N5)/3</f>
+        <f t="shared" si="1"/>
         <v>0.57925567148273427</v>
       </c>
-      <c r="Q5" s="37">
+      <c r="Q5" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -2413,13 +2371,13 @@
         <v>0</v>
       </c>
       <c r="G6" s="15">
-        <f>SUM(B6:E6)/3</f>
+        <f t="shared" si="0"/>
         <v>0.72230376145423703</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="27">
         <v>8</v>
       </c>
-      <c r="I6" s="21"/>
+      <c r="I6" s="18"/>
       <c r="J6" s="5" t="s">
         <v>9</v>
       </c>
@@ -2439,14 +2397,14 @@
         <v>0</v>
       </c>
       <c r="P6" s="15">
-        <f>SUM(K6:N6)/3</f>
+        <f t="shared" si="1"/>
         <v>0.53067829141409406</v>
       </c>
-      <c r="Q6" s="32">
+      <c r="Q6" s="28">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -2466,13 +2424,13 @@
         <v>0</v>
       </c>
       <c r="G7" s="15">
-        <f>SUM(B7:E7)/3</f>
+        <f t="shared" si="0"/>
         <v>0.76323671061713194</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="18">
         <v>6</v>
       </c>
-      <c r="I7" s="21"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="5" t="s">
         <v>16</v>
       </c>
@@ -2492,14 +2450,14 @@
         <v>0</v>
       </c>
       <c r="P7" s="15">
-        <f>SUM(K7:N7)/3</f>
+        <f t="shared" si="1"/>
         <v>0.56997871363484731</v>
       </c>
-      <c r="Q7" s="37">
+      <c r="Q7" s="18">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2519,13 +2477,13 @@
         <v>0</v>
       </c>
       <c r="G8" s="15">
-        <f>SUM(B8:E8)/3</f>
+        <f t="shared" si="0"/>
         <v>0.80321934385409699</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="24">
         <v>2</v>
       </c>
-      <c r="I8" s="21"/>
+      <c r="I8" s="18"/>
       <c r="J8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2545,15 +2503,15 @@
         <v>0</v>
       </c>
       <c r="P8" s="15">
-        <f>SUM(K8:N8)/3</f>
+        <f t="shared" si="1"/>
         <v>0.63698403182054042</v>
       </c>
-      <c r="Q8" s="28">
+      <c r="Q8" s="25">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
-      <c r="A9" s="34" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="12">
@@ -2572,14 +2530,14 @@
         <v>0</v>
       </c>
       <c r="G9" s="15">
-        <f>SUM(B9:E9)/3</f>
+        <f t="shared" si="0"/>
         <v>0.79080307848068998</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9" s="18">
         <v>4</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="34" t="s">
+      <c r="I9" s="18"/>
+      <c r="J9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K9" s="12">
@@ -2598,14 +2556,14 @@
         <v>0</v>
       </c>
       <c r="P9" s="15">
-        <f>SUM(K9:N9)/3</f>
+        <f t="shared" si="1"/>
         <v>0.60836263479583075</v>
       </c>
-      <c r="Q9" s="40">
+      <c r="Q9" s="19">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -2625,13 +2583,13 @@
         <v>0</v>
       </c>
       <c r="G10" s="15">
-        <f>SUM(B10:E10)/3</f>
+        <f t="shared" si="0"/>
         <v>0.7723365058245103</v>
       </c>
-      <c r="H10" s="37">
+      <c r="H10" s="18">
         <v>5</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="18"/>
       <c r="J10" s="5" t="s">
         <v>11</v>
       </c>
@@ -2651,14 +2609,14 @@
         <v>0</v>
       </c>
       <c r="P10" s="15">
-        <f>SUM(K10:N10)/3</f>
+        <f t="shared" si="1"/>
         <v>0.56487460044012028</v>
       </c>
-      <c r="Q10" s="32">
+      <c r="Q10" s="28">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
@@ -2678,13 +2636,13 @@
         <v>0</v>
       </c>
       <c r="G11" s="15">
-        <f>SUM(B11:E11)/3</f>
+        <f t="shared" si="0"/>
         <v>0.81246082408341103</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11" s="24">
         <v>1</v>
       </c>
-      <c r="I11" s="21"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="5" t="s">
         <v>6</v>
       </c>
@@ -2704,67 +2662,67 @@
         <v>0</v>
       </c>
       <c r="P11" s="15">
-        <f>SUM(K11:N11)/3</f>
+        <f t="shared" si="1"/>
         <v>0.63821682388021272</v>
       </c>
-      <c r="Q11" s="28">
+      <c r="Q11" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="7" t="str">
-        <f>INDEX($A4:$A10, MATCH(MAX(B4:B10), B4:B10, 0))</f>
+        <f>INDEX($A4:$A11, MATCH(MAX(B4:B11), B4:B11, 0))</f>
         <v>v0-unstruct</v>
       </c>
       <c r="C12" s="7" t="str">
-        <f>INDEX($A4:$A10, MATCH(MAX(C4:C10), C4:C10, 0))</f>
+        <f>INDEX($A4:$A11, MATCH(MAX(C4:C11), C4:C11, 0))</f>
         <v>v2-json</v>
       </c>
       <c r="D12" s="7" t="str">
-        <f>INDEX($A4:$A10, MATCH(MAX(D4:D10), D4:D10, 0))</f>
+        <f>INDEX($A4:$A11, MATCH(MAX(D4:D11), D4:D11, 0))</f>
         <v>v2-json</v>
       </c>
       <c r="E12" s="7" t="str">
-        <f>INDEX($A4:$A10, MATCH(MAX(E4:E10), E4:E10, 0))</f>
+        <f>INDEX($A4:$A11, MATCH(MAX(E4:E11), E4:E11, 0))</f>
         <v>v2-custom1</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="16" t="str">
-        <f>INDEX($A3:$A11, MATCH(MAX(G3:G11), G3:G11, 0))</f>
+        <f>INDEX($A4:$A11, MATCH(MAX(G4:G11), G4:G11, 0))</f>
         <v>v2-toml</v>
       </c>
-      <c r="H12" s="38"/>
+      <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="8"/>
       <c r="K12" s="7" t="str">
-        <f>INDEX($J4:$J10, MATCH(MAX(K4:K10), K4:K10, 0))</f>
+        <f>INDEX($J4:$J11, MATCH(MAX(K4:K11), K4:K11, 0))</f>
         <v>v0-unstruct</v>
       </c>
       <c r="L12" s="7" t="str">
-        <f>INDEX($J4:$J10, MATCH(MAX(L4:L10), L4:L10, 0))</f>
+        <f t="shared" ref="L12:N12" si="2">INDEX($J4:$J11, MATCH(MAX(L4:L11), L4:L11, 0))</f>
+        <v>v2-toml</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f t="shared" si="2"/>
         <v>v2-json</v>
       </c>
-      <c r="M12" s="7" t="str">
-        <f>INDEX($J4:$J10, MATCH(MAX(M4:M10), M4:M10, 0))</f>
-        <v>v2-json</v>
-      </c>
       <c r="N12" s="7" t="str">
-        <f>INDEX($J4:$J10, MATCH(MAX(N4:N10), N4:N10, 0))</f>
+        <f t="shared" si="2"/>
         <v>v2-custom1</v>
       </c>
       <c r="O12" s="7"/>
       <c r="P12" s="16" t="str">
-        <f>INDEX($A3:$A11, MATCH(MAX(P3:P11), P3:P11, 0))</f>
+        <f>INDEX($J4:$J11, MATCH(MAX(P4:P11), P4:P11, 0))</f>
         <v>v2-toml</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>26</v>
       </c>
@@ -2777,8 +2735,8 @@
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="L2:P2"/>
   </mergeCells>
-  <conditionalFormatting sqref="K4:N11">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="B4:E11">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2789,8 +2747,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E11">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="K4:N11">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>